<commit_message>
issue #5: add legislator_id, name, date into dataframe
</commit_message>
<xml_diff>
--- a/legislator/property/output/change/丁守中_2013-12-26_變動財產申報表_tmpe3691.xlsx
+++ b/legislator/property/output/change/丁守中_2013-12-26_變動財產申報表_tmpe3691.xlsx
@@ -7,90 +7,16 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="土地" sheetId="1" r:id="rId1"/>
-    <sheet name="股票" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
-  <si>
-    <t>土地</t>
-  </si>
-  <si>
-    <t>坐</t>
-  </si>
-  <si>
-    <t>落</t>
-  </si>
-  <si>
-    <t>面積（平方公尺）</t>
-  </si>
-  <si>
-    <t>權利範圍(持分）</t>
-  </si>
-  <si>
-    <t>所有權人</t>
-  </si>
-  <si>
-    <t>變動時間</t>
-  </si>
-  <si>
-    <t>變動原因</t>
-  </si>
-  <si>
-    <t>變動時之價額</t>
-  </si>
-  <si>
-    <t>名稱</t>
-  </si>
-  <si>
-    <t>證券交易商名稱</t>
-  </si>
-  <si>
-    <t>所有人</t>
-  </si>
-  <si>
-    <t>股數</t>
-  </si>
-  <si>
-    <t>總額</t>
-  </si>
-  <si>
-    <t>琉園</t>
-  </si>
-  <si>
-    <t>元大寶來證券</t>
-  </si>
-  <si>
-    <t>溫子苓</t>
-  </si>
-  <si>
-    <t>101年11月 07日</t>
-  </si>
-  <si>
-    <t>101年11月 08日</t>
-  </si>
-  <si>
-    <t>賣出</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -106,7 +32,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -114,30 +40,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -433,139 +340,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:J1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="2:10">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2">
-        <v>5000</v>
-      </c>
-      <c r="F2" s="2">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="2">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1">
-        <v>25</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2">
-        <v>4000</v>
-      </c>
-      <c r="F3" s="2">
-        <v>16</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="2">
-        <v>64000</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>